<commit_message>
Make Interop Range tests passed
</commit_message>
<xml_diff>
--- a/ExcelProcesser.Tests/resources/test.xlsx
+++ b/ExcelProcesser.Tests/resources/test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21107"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VsCode\Github\ExcelProcesser\ExcelProcesser.Tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA8C7A3-BA52-4DB8-9A5F-2DEA47A6F4A5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="8508" windowHeight="4536" tabRatio="652"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="8508" windowHeight="4536" tabRatio="652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="11" r:id="rId1"/>
@@ -155,7 +156,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="8">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -374,7 +375,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,6 +435,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -726,7 +733,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -756,49 +763,52 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="41">
-    <cellStyle name="??" xfId="1"/>
-    <cellStyle name="?? [0]_SGV" xfId="2"/>
-    <cellStyle name="???[0]_PRESHPY3" xfId="3"/>
-    <cellStyle name="???_PRESHPY3" xfId="4"/>
-    <cellStyle name="??[0]_PRESHPY3" xfId="5"/>
-    <cellStyle name="??_594,2" xfId="6"/>
-    <cellStyle name="?@!Ae_PRESHPY3" xfId="7"/>
-    <cellStyle name="?d?A|i[0]_PRSP121" xfId="8"/>
-    <cellStyle name="?d?A|i_PRSP121" xfId="9"/>
-    <cellStyle name="3f1o[0]_PRESHPY3" xfId="10"/>
-    <cellStyle name="3f1o_PRESHPY3" xfId="11"/>
+    <cellStyle name="??" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="?? [0]_SGV" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="???[0]_PRESHPY3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="???_PRESHPY3" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="??[0]_PRESHPY3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="??_594,2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="?@!Ae_PRESHPY3" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="?d?A|i[0]_PRSP121" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="?d?A|i_PRSP121" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="3f1o[0]_PRESHPY3" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="3f1o_PRESHPY3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Bad" xfId="25" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="32" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="33" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="34" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="30" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Grey" xfId="12"/>
+    <cellStyle name="Grey" xfId="12" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
     <cellStyle name="Heading 1" xfId="21" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="22" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="23" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="24" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Input" xfId="39" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Input [yellow]" xfId="13"/>
+    <cellStyle name="Input [yellow]" xfId="13" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
     <cellStyle name="Linked Cell" xfId="36" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="37" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="14"/>
+    <cellStyle name="Normal - Style1" xfId="14" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="Note" xfId="40" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="38" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent [2]" xfId="15"/>
+    <cellStyle name="Percent [2]" xfId="15" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="Title" xfId="20" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="31" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Tusental (0)_pldt" xfId="16"/>
-    <cellStyle name="Tusental_pldt" xfId="17"/>
-    <cellStyle name="Valuta (0)_pldt" xfId="18"/>
-    <cellStyle name="Valuta_pldt" xfId="19"/>
+    <cellStyle name="Tusental (0)_pldt" xfId="16" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Tusental_pldt" xfId="17" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Valuta (0)_pldt" xfId="18" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="Valuta_pldt" xfId="19" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
     <cellStyle name="Warning Text" xfId="35" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="常规 2" xfId="26"/>
-    <cellStyle name="常规 4" xfId="27"/>
-    <cellStyle name="常规 4 11" xfId="28"/>
-    <cellStyle name="常规 6" xfId="29"/>
+    <cellStyle name="常规 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="常规 4" xfId="27" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="常规 4 11" xfId="28" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="常规 6" xfId="29" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -894,6 +904,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -929,6 +956,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1104,12 +1148,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
@@ -1124,7 +1168,7 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E2" s="11" t="s">

</xml_diff>